<commit_message>
Choix caméra dans programme
</commit_message>
<xml_diff>
--- a/Documents gestion de projet/GanttRVP2.xlsx
+++ b/Documents gestion de projet/GanttRVP2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECL\Module Pro\PAr\PAr-Analyse-vitesse-rotation\Documents gestion de projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EB9697-852E-47B8-B480-A7EE59B82F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F88425-EF24-43B7-A993-3A2EF720D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{0A8F5DF2-32AD-4917-BF70-1B964A6F13A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A8F5DF2-32AD-4917-BF70-1B964A6F13A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Tâches</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Rapport / article</t>
-  </si>
-  <si>
-    <t>Communication extérieure</t>
   </si>
   <si>
     <t>Guillaume</t>
@@ -160,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +190,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -339,11 +344,15 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D5527D-923B-406E-B456-2F39084DC913}">
-  <dimension ref="B1:AH30"/>
+  <dimension ref="B1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AI27" sqref="AI27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,69 +697,67 @@
     <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="34" width="3.33203125" customWidth="1"/>
+    <col min="5" max="32" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20" t="s">
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20" t="s">
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20" t="s">
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20" t="s">
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20" t="s">
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="21"/>
-    </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B3" s="23"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="AF2" s="25"/>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B3" s="27"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="3">
         <v>40</v>
       </c>
@@ -832,17 +839,11 @@
       <c r="AE3" s="3">
         <v>14</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AF3" s="4">
         <v>15</v>
       </c>
-      <c r="AG3" s="3">
-        <v>16</v>
-      </c>
-      <c r="AH3" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -877,11 +878,9 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="4"/>
-    </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF4" s="4"/>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
@@ -916,16 +915,14 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="4"/>
-    </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF5" s="4"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -955,11 +952,9 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="4"/>
-    </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF6" s="4"/>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -991,21 +986,19 @@
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
+      <c r="AC7" s="8"/>
       <c r="AD7" s="8"/>
       <c r="AE7" s="8"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="8"/>
-      <c r="AH7" s="9"/>
-    </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="AF7" s="9"/>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1019,8 +1012,8 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
@@ -1032,34 +1025,32 @@
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="4"/>
-    </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3" t="s">
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="4"/>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
@@ -1072,16 +1063,14 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
       <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="4"/>
-    </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF9" s="4"/>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C10" s="6">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1089,19 +1078,19 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="2"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
+      <c r="V10" s="2"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
@@ -1111,11 +1100,9 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="4"/>
-    </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF10" s="4"/>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
@@ -1125,15 +1112,15 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
@@ -1143,43 +1130,39 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
+      <c r="Y11" s="1"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="4"/>
-    </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF11" s="4"/>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="6">
-        <v>1</v>
-      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="1"/>
@@ -1189,15 +1172,15 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="4"/>
-    </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF12" s="4"/>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.95</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1207,15 +1190,15 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -1226,16 +1209,14 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
       <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="4"/>
-    </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF13" s="4"/>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1243,19 +1224,19 @@
       <c r="G14" s="1"/>
       <c r="H14" s="3"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="3"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="1"/>
@@ -1265,16 +1246,14 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="4"/>
-    </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF14" s="4"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="6">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1285,34 +1264,34 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
-      <c r="AH15" s="4"/>
-    </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="4"/>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1331,99 +1310,95 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="4"/>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
-        <v>37</v>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="4"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="4"/>
-    </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="4"/>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="11"/>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="1"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="4"/>
-    </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF18" s="4"/>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6">
         <v>0</v>
@@ -1446,23 +1421,21 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="11"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
       <c r="Y19" s="1"/>
-      <c r="Z19" s="11"/>
+      <c r="Z19" s="3"/>
       <c r="AA19" s="11"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="4"/>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF19" s="4"/>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C20" s="6">
         <v>0</v>
@@ -1479,34 +1452,32 @@
       <c r="M20" s="3"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="1"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
       <c r="AC20" s="11"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="4"/>
-    </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="4"/>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="D21" s="3"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1516,36 +1487,34 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="3"/>
-      <c r="AA21" s="10"/>
-      <c r="AB21" s="10"/>
-      <c r="AC21" s="11"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="1"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="4"/>
-    </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="4"/>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1554,13 +1523,13 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -1573,17 +1542,13 @@
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="3"/>
-      <c r="AH22" s="4"/>
-    </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF22" s="4"/>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="6">
-        <v>1</v>
-      </c>
+      <c r="C23" s="6"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1593,18 +1558,18 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="13"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
@@ -1612,15 +1577,15 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
       <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
-      <c r="AH23" s="4"/>
-    </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF23" s="4"/>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.5</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1639,9 +1604,9 @@
       <c r="S24" s="14"/>
       <c r="T24" s="14"/>
       <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="3"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
@@ -1649,16 +1614,14 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
-      <c r="AF24" s="3"/>
-      <c r="AG24" s="3"/>
-      <c r="AH24" s="4"/>
-    </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AF24" s="4"/>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1670,17 +1633,17 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="3"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="14"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
@@ -1688,13 +1651,11 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
-      <c r="AH25" s="4"/>
-    </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>31</v>
+      <c r="AF25" s="4"/>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B26" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="C26" s="6">
         <v>0</v>
@@ -1709,35 +1670,31 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="3"/>
       <c r="Y26" s="1"/>
-      <c r="Z26" s="3"/>
+      <c r="Z26" s="14"/>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="4"/>
-    </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
+      <c r="AF26" s="4"/>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B27" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="6">
-        <v>0</v>
-      </c>
+      <c r="C27" s="6"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1759,22 +1716,22 @@
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="3"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="3"/>
-      <c r="AB27" s="3"/>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="3"/>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="3"/>
-      <c r="AG27" s="3"/>
-      <c r="AH27" s="4"/>
-    </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="6"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="14"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="14"/>
+      <c r="AE27" s="14"/>
+      <c r="AF27" s="18"/>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B28" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1791,106 +1748,63 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="14"/>
       <c r="AB28" s="14"/>
-      <c r="AC28" s="14"/>
-      <c r="AD28" s="14"/>
-      <c r="AE28" s="14"/>
-      <c r="AF28" s="14"/>
-      <c r="AG28" s="3"/>
-      <c r="AH28" s="4"/>
-    </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B29" s="7" t="s">
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="4"/>
+    </row>
+    <row r="29" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="15">
         <v>0</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="14"/>
-      <c r="AB29" s="14"/>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
-      <c r="AE29" s="3"/>
-      <c r="AF29" s="3"/>
-      <c r="AG29" s="3"/>
-      <c r="AH29" s="4"/>
-    </row>
-    <row r="30" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="16">
-        <v>0</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17"/>
-      <c r="Y30" s="17"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="17"/>
-      <c r="AB30" s="17"/>
-      <c r="AC30" s="18"/>
-      <c r="AD30" s="18"/>
-      <c r="AE30" s="18"/>
-      <c r="AF30" s="18"/>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="19"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
+      <c r="AA29" s="16"/>
+      <c r="AB29" s="16"/>
+      <c r="AC29" s="17"/>
+      <c r="AD29" s="17"/>
+      <c r="AE29" s="17"/>
+      <c r="AF29" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>

</xml_diff>